<commit_message>
dashboard med bubble chart
</commit_message>
<xml_diff>
--- a/EDA/data/studerande-och-examinerade-inom-smala-yrkesomraden-2014-2024.xlsx
+++ b/EDA/data/studerande-och-examinerade-inom-smala-yrkesomraden-2014-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ira/Documents/DE24/github/the-skool-group5/EDA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699ED5A0-A24B-3643-B37E-01D20DED0859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB9BF5-9B6B-A941-BBFF-F84DD2FC31C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1100" windowWidth="28840" windowHeight="17420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5003,7 +5003,7 @@
   <dimension ref="A1:AC42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="214" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>